<commit_message>
updated files for case study morocco, Not yet optimised to approach results, but adjustable without errors
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
+++ b/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,11 +552,11 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[0. 0. 0. 0.]</t>
+          <t>[35, 35, 35, 35]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>['FC']</t>
+          <t>['SAT']</t>
         </is>
       </c>
     </row>
@@ -611,11 +611,11 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[0. 0. 0. 0.]</t>
+          <t>[35, 35, 35, 35]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>['FC']</t>
+          <t>['SAT']</t>
         </is>
       </c>
     </row>
@@ -670,11 +670,11 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[0. 0. 0. 0.]</t>
+          <t>[35, 35, 35, 35]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -691,361 +691,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>V1</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>31.67778</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-7.59167</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>11/21</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="N5" t="n">
-        <v>180</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>31.68056</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-7.58889</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>11/21</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="N6" t="n">
-        <v>180</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>V3</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>31.68056</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-7.59861</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>12/15</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="N7" t="n">
-        <v>180</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>V4</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>31.68056</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-7.59583</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>12/19</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="N8" t="n">
-        <v>180</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>V5</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>31.68056</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-7.59167</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>12/20</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="N9" t="n">
-        <v>180</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>['FC']</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>V6</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>31.66667</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-7.61111</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>38353</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>39082</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>ClayLoam</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>12/24</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>[0. 0. 0. 0.]</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Prop</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="N10" t="n">
-        <v>180</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>['FC']</t>
+          <t>['SAT']</t>
         </is>
       </c>
     </row>
@@ -1060,7 +706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1120,16 +766,16 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>38864</v>
+        <v>38900</v>
       </c>
       <c r="E2" t="n">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="F2" t="n">
-        <v>1.210418098684268</v>
+        <v>10.17405386846855</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>675</v>
       </c>
     </row>
     <row r="3">
@@ -1147,16 +793,16 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>38484</v>
+        <v>38560</v>
       </c>
       <c r="E3" t="n">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>10.30989602463866</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>925</v>
       </c>
     </row>
     <row r="4">
@@ -1174,16 +820,16 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>38864</v>
+        <v>38925</v>
       </c>
       <c r="E4" t="n">
-        <v>510</v>
+        <v>571</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1284225563411552</v>
+        <v>10.44909636758182</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>825</v>
       </c>
     </row>
     <row r="5">
@@ -1201,16 +847,16 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>38485</v>
+        <v>38563</v>
       </c>
       <c r="E5" t="n">
-        <v>131</v>
+        <v>209</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>10.34309105783272</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>950</v>
       </c>
     </row>
     <row r="6">
@@ -1228,178 +874,16 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>38866</v>
+        <v>38928</v>
       </c>
       <c r="E6" t="n">
-        <v>512</v>
+        <v>574</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0906134738812487</v>
+        <v>10.46557734423419</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>V1</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>38874</v>
-      </c>
-      <c r="E7" t="n">
-        <v>520</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.89805990585905</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>38874</v>
-      </c>
-      <c r="E8" t="n">
-        <v>520</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3.898827943600271</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>V3</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>38866</v>
-      </c>
-      <c r="E9" t="n">
-        <v>512</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.461858091781556</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>V4</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>38866</v>
-      </c>
-      <c r="E10" t="n">
-        <v>512</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.175535701629666</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>V5</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>38866</v>
-      </c>
-      <c r="E11" t="n">
-        <v>512</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.109881684506034</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>V6</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>38864</v>
-      </c>
-      <c r="E12" t="n">
-        <v>510</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.7685788956099961</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
+        <v>825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everything regarding aquacrop sim for jip has been updated. cleaned up. added some water related files. and general nicer structure
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
+++ b/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +534,7 @@
         <v>38353</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>39082</v>
+        <v>42369</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -552,11 +552,11 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -573,7 +573,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>['SAT']</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
         <v>38353</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>39082</v>
+        <v>42004</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -611,11 +611,11 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>['SAT']</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
         <v>38353</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>39082</v>
+        <v>42004</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -670,11 +670,11 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -691,7 +691,361 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>['SAT']</t>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>31.67778</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-7.59167</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>11/21</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="N5" t="n">
+        <v>180</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>31.68056</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-7.58889</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>11/21</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="N6" t="n">
+        <v>180</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>31.68056</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-7.59861</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>12/15</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="N7" t="n">
+        <v>180</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>31.68056</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-7.59583</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>12/19</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="N8" t="n">
+        <v>180</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>31.68056</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-7.59167</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>12/20</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="N9" t="n">
+        <v>180</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>['FC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>31.66667</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-7.61111</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>38353</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>42369</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ClayLoam</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>12/24</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>[0. 0. 0. 0.]</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Prop</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="N10" t="n">
+        <v>180</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -706,7 +1060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,26 +1120,26 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>38900</v>
+        <v>38867</v>
       </c>
       <c r="E2" t="n">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="F2" t="n">
-        <v>10.17405386846855</v>
+        <v>1.579942260272885</v>
       </c>
       <c r="G2" t="n">
-        <v>675</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -793,26 +1147,26 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>38560</v>
+        <v>39233</v>
       </c>
       <c r="E3" t="n">
-        <v>206</v>
+        <v>879</v>
       </c>
       <c r="F3" t="n">
-        <v>10.30989602463866</v>
+        <v>1.388958882316788</v>
       </c>
       <c r="G3" t="n">
-        <v>925</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -820,26 +1174,26 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>38925</v>
+        <v>39592</v>
       </c>
       <c r="E4" t="n">
-        <v>571</v>
+        <v>1238</v>
       </c>
       <c r="F4" t="n">
-        <v>10.44909636758182</v>
+        <v>1.041122702504644</v>
       </c>
       <c r="G4" t="n">
-        <v>825</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -847,43 +1201,2338 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>38563</v>
+        <v>39959</v>
       </c>
       <c r="E5" t="n">
-        <v>209</v>
+        <v>1605</v>
       </c>
       <c r="F5" t="n">
-        <v>10.34309105783272</v>
+        <v>1.568932260684225</v>
       </c>
       <c r="G5" t="n">
-        <v>950</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>40329</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1975</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.921708687464276</v>
+      </c>
+      <c r="G6" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>40723</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2369</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.890158769836202</v>
+      </c>
+      <c r="G7" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>41057</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2703</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.493771469026509</v>
+      </c>
+      <c r="G8" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>41417</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3063</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.028879862705715</v>
+      </c>
+      <c r="G9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>41784</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3430</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.289317735065304</v>
+      </c>
+      <c r="G10" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>42156</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3802</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.504375476468089</v>
+      </c>
+      <c r="G11" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>38509</v>
+      </c>
+      <c r="E12" t="n">
+        <v>155</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4363535815396039</v>
+      </c>
+      <c r="G12" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>38878</v>
+      </c>
+      <c r="E13" t="n">
+        <v>524</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6793167828313862</v>
+      </c>
+      <c r="G13" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>39243</v>
+      </c>
+      <c r="E14" t="n">
+        <v>889</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.7280668304257699</v>
+      </c>
+      <c r="G14" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>39605</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1251</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4604396575147147</v>
+      </c>
+      <c r="G15" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>39975</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1621</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9028831886863407</v>
+      </c>
+      <c r="G16" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>40337</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1983</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5599204253154705</v>
+      </c>
+      <c r="G17" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>40731</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2377</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3.266490734042698</v>
+      </c>
+      <c r="G18" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>7</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>41074</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2720</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.22161814925332</v>
+      </c>
+      <c r="G19" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>8</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>41434</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3080</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.7251071554837019</v>
+      </c>
+      <c r="G20" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>9</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>41803</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3449</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.9722379560448858</v>
+      </c>
+      <c r="G21" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>C3</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>38505</v>
+      </c>
+      <c r="E22" t="n">
+        <v>151</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1838874688288261</v>
+      </c>
+      <c r="G22" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Wheat</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>38928</v>
-      </c>
-      <c r="E6" t="n">
-        <v>574</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10.46557734423419</v>
-      </c>
-      <c r="G6" t="n">
-        <v>825</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>38901</v>
+      </c>
+      <c r="E23" t="n">
+        <v>547</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.690732715774311</v>
+      </c>
+      <c r="G23" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>39240</v>
+      </c>
+      <c r="E24" t="n">
+        <v>886</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.3280214592659579</v>
+      </c>
+      <c r="G24" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>39601</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1247</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.19031993139703</v>
+      </c>
+      <c r="G25" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>39972</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1618</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.4059816304621579</v>
+      </c>
+      <c r="G26" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>40336</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1982</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.3581045100035088</v>
+      </c>
+      <c r="G27" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>40730</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2376</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.43953874431695</v>
+      </c>
+      <c r="G28" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>7</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>41072</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2718</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.6549529034558902</v>
+      </c>
+      <c r="G29" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>8</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>41430</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3076</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.2743477914405739</v>
+      </c>
+      <c r="G30" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>9</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>41796</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3442</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.3106031964156856</v>
+      </c>
+      <c r="G31" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>38871</v>
+      </c>
+      <c r="E32" t="n">
+        <v>517</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5.90203502256449</v>
+      </c>
+      <c r="G32" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>39234</v>
+      </c>
+      <c r="E33" t="n">
+        <v>880</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.461549507073756</v>
+      </c>
+      <c r="G33" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>39588</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.527454198831712</v>
+      </c>
+      <c r="G34" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>39961</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1607</v>
+      </c>
+      <c r="F35" t="n">
+        <v>5.458805849164687</v>
+      </c>
+      <c r="G35" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>40334</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F36" t="n">
+        <v>6.36358215205555</v>
+      </c>
+      <c r="G36" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>40700</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2346</v>
+      </c>
+      <c r="F37" t="n">
+        <v>6.222372956223233</v>
+      </c>
+      <c r="G37" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>6</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>41060</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2706</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5.076218177768834</v>
+      </c>
+      <c r="G38" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>7</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>41412</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3058</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3.620546570623358</v>
+      </c>
+      <c r="G39" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>8</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>41782</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3428</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.676399366771229</v>
+      </c>
+      <c r="G40" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>9</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>42145</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3791</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.127346185184509</v>
+      </c>
+      <c r="G41" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>38869</v>
+      </c>
+      <c r="E42" t="n">
+        <v>515</v>
+      </c>
+      <c r="F42" t="n">
+        <v>5.591678365857279</v>
+      </c>
+      <c r="G42" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>39234</v>
+      </c>
+      <c r="E43" t="n">
+        <v>880</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4.502776349511979</v>
+      </c>
+      <c r="G43" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>39587</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1233</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3.545331062289606</v>
+      </c>
+      <c r="G44" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>39960</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1606</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5.269474237511353</v>
+      </c>
+      <c r="G45" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>40334</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F46" t="n">
+        <v>6.147181577977309</v>
+      </c>
+      <c r="G46" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>40700</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2346</v>
+      </c>
+      <c r="F47" t="n">
+        <v>6.095494134339486</v>
+      </c>
+      <c r="G47" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>6</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>41060</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2706</v>
+      </c>
+      <c r="F48" t="n">
+        <v>5.161731870455706</v>
+      </c>
+      <c r="G48" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>7</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>41410</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3056</v>
+      </c>
+      <c r="F49" t="n">
+        <v>3.396316656408048</v>
+      </c>
+      <c r="G49" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>8</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>41796</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3442</v>
+      </c>
+      <c r="F50" t="n">
+        <v>5.945525312497332</v>
+      </c>
+      <c r="G50" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>9</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>42142</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3788</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3.867646959422582</v>
+      </c>
+      <c r="G51" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>38868</v>
+      </c>
+      <c r="E52" t="n">
+        <v>514</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2.183680160436081</v>
+      </c>
+      <c r="G52" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>39235</v>
+      </c>
+      <c r="E53" t="n">
+        <v>881</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2.180376595526162</v>
+      </c>
+      <c r="G53" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>39588</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1.283574680467467</v>
+      </c>
+      <c r="G54" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>3</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>39962</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1608</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2.325437553377062</v>
+      </c>
+      <c r="G55" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>40334</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1980</v>
+      </c>
+      <c r="F56" t="n">
+        <v>2.684148207221433</v>
+      </c>
+      <c r="G56" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>5</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>40724</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2370</v>
+      </c>
+      <c r="F57" t="n">
+        <v>5.362007912699632</v>
+      </c>
+      <c r="G57" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>6</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>41058</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2704</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2.307544581514701</v>
+      </c>
+      <c r="G58" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>7</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>41426</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3072</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2.417651058829135</v>
+      </c>
+      <c r="G59" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>8</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>41783</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3429</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1.871937624569682</v>
+      </c>
+      <c r="G60" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>9</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>42147</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3793</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1.583195640300309</v>
+      </c>
+      <c r="G61" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>38902</v>
+      </c>
+      <c r="E62" t="n">
+        <v>548</v>
+      </c>
+      <c r="F62" t="n">
+        <v>4.355552653827536</v>
+      </c>
+      <c r="G62" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>39242</v>
+      </c>
+      <c r="E63" t="n">
+        <v>888</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2.343869402602802</v>
+      </c>
+      <c r="G63" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>39601</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1247</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1.769786255485436</v>
+      </c>
+      <c r="G64" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>39971</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1617</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2.742125069036561</v>
+      </c>
+      <c r="G65" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>4</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>40336</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1982</v>
+      </c>
+      <c r="F66" t="n">
+        <v>2.617726656675007</v>
+      </c>
+      <c r="G66" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>5</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>40728</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2374</v>
+      </c>
+      <c r="F67" t="n">
+        <v>5.530781641713832</v>
+      </c>
+      <c r="G67" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>6</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>41067</v>
+      </c>
+      <c r="E68" t="n">
+        <v>2713</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2.550629493210427</v>
+      </c>
+      <c r="G68" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>7</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>41431</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3077</v>
+      </c>
+      <c r="F69" t="n">
+        <v>2.383655850262514</v>
+      </c>
+      <c r="G69" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>8</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>41796</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3442</v>
+      </c>
+      <c r="F70" t="n">
+        <v>2.409651672230105</v>
+      </c>
+      <c r="G70" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>V4</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>9</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>42160</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3806</v>
+      </c>
+      <c r="F71" t="n">
+        <v>2.137900149929369</v>
+      </c>
+      <c r="G71" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>38868</v>
+      </c>
+      <c r="E72" t="n">
+        <v>514</v>
+      </c>
+      <c r="F72" t="n">
+        <v>1.604348204776908</v>
+      </c>
+      <c r="G72" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>39234</v>
+      </c>
+      <c r="E73" t="n">
+        <v>880</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1.577996600126307</v>
+      </c>
+      <c r="G73" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>39588</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.8072661063805969</v>
+      </c>
+      <c r="G74" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>39962</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1608</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1.79643661644939</v>
+      </c>
+      <c r="G75" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>4</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>40321</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1967</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1.2083957287072</v>
+      </c>
+      <c r="G76" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>5</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>40729</v>
+      </c>
+      <c r="E77" t="n">
+        <v>2375</v>
+      </c>
+      <c r="F77" t="n">
+        <v>5.009201567124835</v>
+      </c>
+      <c r="G77" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>6</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>41061</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2707</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1.97614921683898</v>
+      </c>
+      <c r="G78" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>7</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>41419</v>
+      </c>
+      <c r="E79" t="n">
+        <v>3065</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.298891032664264</v>
+      </c>
+      <c r="G79" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>8</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>41785</v>
+      </c>
+      <c r="E80" t="n">
+        <v>3431</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1.426967354816996</v>
+      </c>
+      <c r="G80" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>V5</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>9</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>42149</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3795</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.269020196314903</v>
+      </c>
+      <c r="G81" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>38867</v>
+      </c>
+      <c r="E82" t="n">
+        <v>513</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1.122072197659475</v>
+      </c>
+      <c r="G82" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>39234</v>
+      </c>
+      <c r="E83" t="n">
+        <v>880</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1.347360329256473</v>
+      </c>
+      <c r="G83" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>2</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>39588</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.5634612205370853</v>
+      </c>
+      <c r="G84" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>39964</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1610</v>
+      </c>
+      <c r="F85" t="n">
+        <v>1.592923812366729</v>
+      </c>
+      <c r="G85" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>4</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>40320</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1966</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.6982297921730262</v>
+      </c>
+      <c r="G86" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>5</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>40724</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2370</v>
+      </c>
+      <c r="F87" t="n">
+        <v>4.202080396486859</v>
+      </c>
+      <c r="G87" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>6</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="n">
+        <v>41061</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2707</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1.681159076009684</v>
+      </c>
+      <c r="G88" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>7</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>41427</v>
+      </c>
+      <c r="E89" t="n">
+        <v>3073</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1.572987050198307</v>
+      </c>
+      <c r="G89" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>8</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>41787</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3433</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1.22923949205622</v>
+      </c>
+      <c r="G90" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>9</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>42150</v>
+      </c>
+      <c r="E91" t="n">
+        <v>3796</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.9803944803571764</v>
+      </c>
+      <c r="G91" t="n">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
morroco casestudy update and fix results bangalade
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
+++ b/heliostrome/jip_project/results/test_results_moroccoWheat.xlsx
@@ -525,10 +525,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31.66111</v>
+        <v>31.68056</v>
       </c>
       <c r="C2" t="n">
-        <v>-7.60972</v>
+        <v>-7.59583</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>38718</v>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>31.66667</v>
+        <v>31.68056</v>
       </c>
       <c r="C3" t="n">
-        <v>-7.59167</v>
+        <v>-7.59583</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>38353</v>
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31.66806</v>
+        <v>31.68056</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.59444</v>
+        <v>-7.59583</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>38353</v>
@@ -702,10 +702,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>31.67778</v>
+        <v>31.68056</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.59167</v>
+        <v>-7.59583</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>38718</v>
@@ -764,7 +764,7 @@
         <v>31.68056</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.58889</v>
+        <v>-7.59583</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>38718</v>
@@ -823,7 +823,7 @@
         <v>31.68056</v>
       </c>
       <c r="C7" t="n">
-        <v>-7.59861</v>
+        <v>-7.59583</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>38718</v>
@@ -941,7 +941,7 @@
         <v>31.68056</v>
       </c>
       <c r="C9" t="n">
-        <v>-7.59167</v>
+        <v>-7.59583</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>38718</v>
@@ -997,10 +997,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>31.66667</v>
+        <v>31.68056</v>
       </c>
       <c r="C10" t="n">
-        <v>-7.61111</v>
+        <v>-7.59583</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>38718</v>
@@ -1120,13 +1120,13 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>39233</v>
+        <v>39234</v>
       </c>
       <c r="E2" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F2" t="n">
-        <v>1.388390010308154</v>
+        <v>1.52859279853724</v>
       </c>
       <c r="G2" t="n">
         <v>90</v>
@@ -1147,13 +1147,13 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>39592</v>
+        <v>39590</v>
       </c>
       <c r="E3" t="n">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="F3" t="n">
-        <v>1.042147171659506</v>
+        <v>1.027367046393602</v>
       </c>
       <c r="G3" t="n">
         <v>90</v>
@@ -1180,7 +1180,7 @@
         <v>1240</v>
       </c>
       <c r="F4" t="n">
-        <v>1.570123335144083</v>
+        <v>1.568234878753612</v>
       </c>
       <c r="G4" t="n">
         <v>90</v>
@@ -1201,13 +1201,13 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>40329</v>
+        <v>40333</v>
       </c>
       <c r="E5" t="n">
-        <v>1610</v>
+        <v>1614</v>
       </c>
       <c r="F5" t="n">
-        <v>1.923809078388547</v>
+        <v>2.153246342067261</v>
       </c>
       <c r="G5" t="n">
         <v>90</v>
@@ -1234,7 +1234,7 @@
         <v>155</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4345764467816526</v>
+        <v>0.4341064463304053</v>
       </c>
       <c r="G6" t="n">
         <v>180</v>
@@ -1261,7 +1261,7 @@
         <v>524</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6797842236821868</v>
+        <v>0.6792629133508745</v>
       </c>
       <c r="G7" t="n">
         <v>180</v>
@@ -1288,7 +1288,7 @@
         <v>889</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7288608272491159</v>
+        <v>0.72784282473241</v>
       </c>
       <c r="G8" t="n">
         <v>180</v>
@@ -1315,7 +1315,7 @@
         <v>1251</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4603808994384621</v>
+        <v>0.4597446247869066</v>
       </c>
       <c r="G9" t="n">
         <v>180</v>
@@ -1342,7 +1342,7 @@
         <v>1621</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9032792018684389</v>
+        <v>0.9020416044696654</v>
       </c>
       <c r="G10" t="n">
         <v>180</v>
@@ -1369,7 +1369,7 @@
         <v>151</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1832184586259029</v>
+        <v>0.1831497061510858</v>
       </c>
       <c r="G11" t="n">
         <v>120</v>
@@ -1396,7 +1396,7 @@
         <v>547</v>
       </c>
       <c r="F12" t="n">
-        <v>1.691721050092369</v>
+        <v>1.691118173936799</v>
       </c>
       <c r="G12" t="n">
         <v>120</v>
@@ -1423,7 +1423,7 @@
         <v>886</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3284009959798029</v>
+        <v>0.3280135870771285</v>
       </c>
       <c r="G13" t="n">
         <v>120</v>
@@ -1450,7 +1450,7 @@
         <v>1247</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1903858196038916</v>
+        <v>0.1901580738977416</v>
       </c>
       <c r="G14" t="n">
         <v>120</v>
@@ -1477,7 +1477,7 @@
         <v>1618</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4060754650469243</v>
+        <v>0.4056849792480352</v>
       </c>
       <c r="G15" t="n">
         <v>120</v>
@@ -1504,7 +1504,7 @@
         <v>515</v>
       </c>
       <c r="F16" t="n">
-        <v>4.463713627079782</v>
+        <v>4.460284187979638</v>
       </c>
       <c r="G16" t="n">
         <v>180</v>
@@ -1531,7 +1531,7 @@
         <v>869</v>
       </c>
       <c r="F17" t="n">
-        <v>3.53091181199222</v>
+        <v>3.527925250845044</v>
       </c>
       <c r="G17" t="n">
         <v>180</v>
@@ -1558,7 +1558,7 @@
         <v>1242</v>
       </c>
       <c r="F18" t="n">
-        <v>5.460048819204386</v>
+        <v>5.458218752051685</v>
       </c>
       <c r="G18" t="n">
         <v>180</v>
@@ -1585,7 +1585,7 @@
         <v>1615</v>
       </c>
       <c r="F19" t="n">
-        <v>6.367971626279126</v>
+        <v>6.36593828368605</v>
       </c>
       <c r="G19" t="n">
         <v>180</v>
@@ -1612,7 +1612,7 @@
         <v>515</v>
       </c>
       <c r="F20" t="n">
-        <v>4.504653428580114</v>
+        <v>4.501058327880293</v>
       </c>
       <c r="G20" t="n">
         <v>180</v>
@@ -1639,7 +1639,7 @@
         <v>868</v>
       </c>
       <c r="F21" t="n">
-        <v>3.549447194064212</v>
+        <v>3.545589493487691</v>
       </c>
       <c r="G21" t="n">
         <v>180</v>
@@ -1666,7 +1666,7 @@
         <v>1241</v>
       </c>
       <c r="F22" t="n">
-        <v>5.270741040481486</v>
+        <v>5.270495471766091</v>
       </c>
       <c r="G22" t="n">
         <v>180</v>
@@ -1693,7 +1693,7 @@
         <v>1615</v>
       </c>
       <c r="F23" t="n">
-        <v>6.151680268321231</v>
+        <v>6.147844923512341</v>
       </c>
       <c r="G23" t="n">
         <v>180</v>
@@ -1720,7 +1720,7 @@
         <v>516</v>
       </c>
       <c r="F24" t="n">
-        <v>2.179788501001285</v>
+        <v>2.179977272884304</v>
       </c>
       <c r="G24" t="n">
         <v>180</v>
@@ -1747,7 +1747,7 @@
         <v>869</v>
       </c>
       <c r="F25" t="n">
-        <v>1.284020434698184</v>
+        <v>1.284153232224922</v>
       </c>
       <c r="G25" t="n">
         <v>180</v>
@@ -1774,7 +1774,7 @@
         <v>1243</v>
       </c>
       <c r="F26" t="n">
-        <v>2.32629045831344</v>
+        <v>2.325970261920851</v>
       </c>
       <c r="G26" t="n">
         <v>180</v>
@@ -1801,7 +1801,7 @@
         <v>1615</v>
       </c>
       <c r="F27" t="n">
-        <v>2.685456597251745</v>
+        <v>2.685650868725979</v>
       </c>
       <c r="G27" t="n">
         <v>180</v>
@@ -1936,7 +1936,7 @@
         <v>515</v>
       </c>
       <c r="F32" t="n">
-        <v>1.576733198107896</v>
+        <v>1.575718291759458</v>
       </c>
       <c r="G32" t="n">
         <v>180</v>
@@ -1963,7 +1963,7 @@
         <v>869</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8075865550571288</v>
+        <v>0.807216653698976</v>
       </c>
       <c r="G33" t="n">
         <v>180</v>
@@ -1990,7 +1990,7 @@
         <v>1243</v>
       </c>
       <c r="F34" t="n">
-        <v>1.796298012145082</v>
+        <v>1.796068706048071</v>
       </c>
       <c r="G34" t="n">
         <v>180</v>
@@ -2017,7 +2017,7 @@
         <v>1602</v>
       </c>
       <c r="F35" t="n">
-        <v>1.209415536587004</v>
+        <v>1.209034815115379</v>
       </c>
       <c r="G35" t="n">
         <v>180</v>
@@ -2038,13 +2038,13 @@
         </is>
       </c>
       <c r="D36" s="3" t="n">
-        <v>39234</v>
+        <v>39235</v>
       </c>
       <c r="E36" t="n">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F36" t="n">
-        <v>1.346730399092992</v>
+        <v>1.353213898001245</v>
       </c>
       <c r="G36" t="n">
         <v>180</v>
@@ -2065,13 +2065,13 @@
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>39588</v>
+        <v>39590</v>
       </c>
       <c r="E37" t="n">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5636963795658604</v>
+        <v>0.7013404472768289</v>
       </c>
       <c r="G37" t="n">
         <v>180</v>
@@ -2092,13 +2092,13 @@
         </is>
       </c>
       <c r="D38" s="3" t="n">
-        <v>39964</v>
+        <v>39965</v>
       </c>
       <c r="E38" t="n">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="F38" t="n">
-        <v>1.593167298090087</v>
+        <v>1.603871174019468</v>
       </c>
       <c r="G38" t="n">
         <v>180</v>
@@ -2119,13 +2119,13 @@
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>40320</v>
+        <v>40322</v>
       </c>
       <c r="E39" t="n">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6987609748670905</v>
+        <v>0.8425797837352049</v>
       </c>
       <c r="G39" t="n">
         <v>180</v>

</xml_diff>